<commit_message>
Update all HCVN nugg
</commit_message>
<xml_diff>
--- a/SAPLINK/projects/HCVN/Packages List.xlsx
+++ b/SAPLINK/projects/HCVN/Packages List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61b59f9583074f6e/14.GitHub/Tuannh1311/SAP/SAPLINK/projects/HCVN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{25453CA5-F177-4F7E-957C-CD5820E5C7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07C96DEF-82A8-40F6-B302-4B5201E8020F}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{25453CA5-F177-4F7E-957C-CD5820E5C7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE8B949D-E021-409F-8558-7E623B1CF185}"/>
   <bookViews>
     <workbookView xWindow="5190" yWindow="1230" windowWidth="20805" windowHeight="13380" xr2:uid="{2E9EA24D-1B08-449D-A364-0BD932FB913B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="160">
   <si>
     <t>SAP</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>HCVN_ZVNWF</t>
+  </si>
+  <si>
+    <t>HCVN_ZABAP_UTIL</t>
+  </si>
+  <si>
+    <t>HCVN_ZABAPGIT</t>
+  </si>
+  <si>
+    <t>HCVN_ZBC_ACTIVITY_LOG</t>
+  </si>
+  <si>
+    <t>HCVN_ZBC_GENERAL</t>
   </si>
 </sst>
 </file>
@@ -528,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +577,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -593,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -601,6 +619,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0457935B-0C6A-4885-8513-E661B3CCB24F}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,64 +967,72 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="7" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1437,7 +1464,7 @@
       <c r="D31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1454,7 +1481,7 @@
       <c r="D32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="3" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1471,7 +1498,7 @@
       <c r="D33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1488,7 +1515,7 @@
       <c r="D34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="3" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1505,7 +1532,7 @@
       <c r="D35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1522,7 +1549,7 @@
       <c r="D36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1539,7 +1566,7 @@
       <c r="D37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1556,7 +1583,7 @@
       <c r="D38" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1573,7 +1600,7 @@
       <c r="D39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1590,7 +1617,7 @@
       <c r="D40" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1607,7 +1634,7 @@
       <c r="D41" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1624,7 +1651,7 @@
       <c r="D42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="3" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1641,7 +1668,7 @@
       <c r="D43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1658,7 +1685,7 @@
       <c r="D44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1675,7 +1702,7 @@
       <c r="D45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1692,7 +1719,7 @@
       <c r="D46" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1709,7 +1736,7 @@
       <c r="D47" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1726,7 +1753,7 @@
       <c r="D48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1743,7 +1770,7 @@
       <c r="D49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1760,24 +1787,24 @@
       <c r="D50" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="B51" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="6" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1809,7 +1836,7 @@
       <c r="D53" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="3" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>